<commit_message>
Restrucure solution projects forPOM.
</commit_message>
<xml_diff>
--- a/Tests/Browsers.xlsx
+++ b/Tests/Browsers.xlsx
@@ -12,7 +12,7 @@
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="BrowserNames" sheetId="10" r:id="rId1"/>
+    <sheet name="Browser" sheetId="10" r:id="rId1"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,30 +24,27 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+  <si>
+    <t>IE</t>
+  </si>
+  <si>
+    <t>CHROME_HEADLESS</t>
+  </si>
+  <si>
+    <t>CHROME</t>
+  </si>
+  <si>
+    <t>EDGE</t>
+  </si>
+  <si>
+    <t>FIREFOX</t>
+  </si>
+  <si>
+    <t>FIREFOX_HEADLESS</t>
+  </si>
   <si>
     <t>BrowserName</t>
-  </si>
-  <si>
-    <t>IE</t>
-  </si>
-  <si>
-    <t>PHANTOMJS_HEADLESS</t>
-  </si>
-  <si>
-    <t>CHROME_HEADLESS</t>
-  </si>
-  <si>
-    <t>CHROME</t>
-  </si>
-  <si>
-    <t>EDGE</t>
-  </si>
-  <si>
-    <t>FIREFOX</t>
-  </si>
-  <si>
-    <t>FIREFOX_HEADLESS</t>
   </si>
 </sst>
 </file>
@@ -399,9 +396,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{15149D48-65BC-4780-8CF3-C741850F6BCC}">
-  <dimension ref="A1:A8"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -410,42 +409,37 @@
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>6</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>